<commit_message>
rgb to ycbcr fixed point implemented
</commit_message>
<xml_diff>
--- a/RGB to YCbCr conversion calculation.xlsx
+++ b/RGB to YCbCr conversion calculation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15920" yWindow="0" windowWidth="11540" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="1160" yWindow="660" windowWidth="26160" windowHeight="8640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Red</t>
   </si>
@@ -37,19 +37,49 @@
   </si>
   <si>
     <t>Cr</t>
+  </si>
+  <si>
+    <t>Inverse</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -70,13 +100,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -406,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -427,42 +461,95 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
+    <row r="5" spans="1:3">
+      <c r="A5">
         <f>16 + (65.481*A2 + 128.553*B2 + 24.966*C2)/255</f>
-        <v>54.681411764705885</v>
-      </c>
-      <c r="B7">
+        <v>16.504129411764705</v>
+      </c>
+      <c r="B5">
         <f>128+(-37.797*A2-74.203*B2+112*C2)/255</f>
-        <v>137.39902745098038</v>
-      </c>
-      <c r="C7">
+        <v>127.70900784313726</v>
+      </c>
+      <c r="C5">
         <f>128+(112*A2-93.786*B2-18.214*C2)/255</f>
-        <v>119.82970980392157</v>
+        <v>127.63221176470589</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>128</v>
+      </c>
+      <c r="C9">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <f>255/219*(A9-16) + 255*0.701/112*(C9-128)</f>
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <f>255/219*(A9-16) - (255/112*0.886*0.114/0.587)*(B9-128) - 255/112*0.701*0.299/0.587*(C9-128)</f>
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <f>255/219*(A9-16)+255/112*0.886*(B9-128)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>